<commit_message>
feat: Update report generation logic to use ExcelJS for improved formatting and add row matching diagnostics
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koaca\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Web\WmsSchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B52470A2-8DB2-41B9-A4CD-6D21BF4CFF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B47DAC-F381-4EE3-9C4A-F0DD7346CAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{F3E83D6E-FE96-42B5-BC21-A1B0BAEED8B4}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="20736" windowHeight="10656" activeTab="1" xr2:uid="{F3E83D6E-FE96-42B5-BC21-A1B0BAEED8B4}"/>
   </bookViews>
   <sheets>
     <sheet name="report" sheetId="1" r:id="rId1"/>
     <sheet name="report_merge" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">report_merge!$A$1:$N$24</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">report_merge!$A$1:$M$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,13 +40,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t xml:space="preserve">B/L </t>
-  </si>
-  <si>
-    <t>KMTCPEN1093885</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -73,10 +69,6 @@
       </rPr>
       <t xml:space="preserve">ty </t>
     </r>
-  </si>
-  <si>
-    <t>토마토 페이스트</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <t>Overage q'ty</t>
@@ -161,22 +153,6 @@
     <t>Damage</t>
   </si>
   <si>
-    <t>MCCU1027470</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>JCSC258278</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>TGHU2845220</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>JCSC291814</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>INSPECTION SHEET</t>
   </si>
   <si>
@@ -195,10 +171,6 @@
       </rPr>
       <t xml:space="preserve">: </t>
     </r>
-  </si>
-  <si>
-    <t>JCSCFE733E008</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
     <r>
@@ -318,7 +290,7 @@
     <numFmt numFmtId="178" formatCode="#,##0.0_ "/>
     <numFmt numFmtId="179" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -437,14 +409,6 @@
       <family val="1"/>
     </font>
     <font>
-      <i/>
-      <u/>
-      <sz val="26"/>
-      <color rgb="FF000000"/>
-      <name val="Bookman Old Style"/>
-      <family val="1"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -481,14 +445,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF474747"/>
-      <name val="Bookman Old Style"/>
-      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -609,7 +565,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="39">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -954,19 +910,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1009,30 +952,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1109,9 +1028,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1175,258 +1094,240 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="41" fontId="25" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="30" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="3" fontId="9" fillId="4" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="32" fillId="4" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="27" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="25" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="3" borderId="26" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="3" borderId="27" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="3" borderId="32" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="32" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="9" fillId="4" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="4" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1453,13 +1354,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1888,13 +1789,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2323,13 +2224,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2758,13 +2659,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3193,13 +3094,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3628,13 +3529,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4063,13 +3964,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4498,13 +4399,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4933,13 +4834,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5368,13 +5269,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5803,13 +5704,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6238,13 +6139,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6673,13 +6574,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -7195,13 +7096,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>1905</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
@@ -8006,10 +7907,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09146C15-1A54-4302-987B-0B0AB35B9D6F}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="B1:I10"/>
+  <dimension ref="B1:I9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.25"/>
@@ -8031,26 +7932,22 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="6">
         <f>SUM(E:E)</f>
-        <v>160</v>
+        <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C4" s="6">
         <f>SUM(H:H)</f>
@@ -8061,7 +7958,7 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="6">
         <f>SUM(F:F)</f>
@@ -8071,7 +7968,7 @@
     </row>
     <row r="6" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C6" s="9">
         <f>SUM(I:I)</f>
@@ -8082,71 +7979,39 @@
     <row r="7" spans="2:9" ht="18" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="2:9" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="E8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="F8" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="H8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="I8" s="13" t="s">
         <v>12</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="15">
-        <v>46021</v>
-      </c>
-      <c r="E9" s="16">
-        <v>80</v>
-      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18"/>
       <c r="H9" s="19"/>
-      <c r="I9" s="18">
-        <f>IFERROR(G9/H9,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="15">
-        <v>46021</v>
-      </c>
-      <c r="E10" s="16">
-        <v>80</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="18">
-        <f>IFERROR(G10/H10,0)</f>
-        <v>0</v>
-      </c>
+      <c r="I9" s="18"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -8160,496 +8025,463 @@
   <sheetPr codeName="Sheet5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10:M11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.59765625" customWidth="1"/>
     <col min="2" max="2" width="12.59765625" customWidth="1"/>
-    <col min="3" max="3" width="8.296875" customWidth="1"/>
-    <col min="4" max="4" width="13.796875" customWidth="1"/>
-    <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="7.8984375" customWidth="1"/>
-    <col min="7" max="7" width="10.296875" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="9" width="7.09765625" customWidth="1"/>
-    <col min="10" max="10" width="14.3984375" customWidth="1"/>
-    <col min="11" max="11" width="6.8984375" customWidth="1"/>
-    <col min="12" max="12" width="6.09765625" customWidth="1"/>
-    <col min="13" max="13" width="5.09765625" customWidth="1"/>
-    <col min="14" max="14" width="15.796875" customWidth="1"/>
+    <col min="3" max="3" width="22.09765625" style="99" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="7.8984375" customWidth="1"/>
+    <col min="6" max="6" width="10.296875" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
+    <col min="8" max="8" width="7.09765625" customWidth="1"/>
+    <col min="9" max="9" width="14.3984375" customWidth="1"/>
+    <col min="10" max="10" width="6.8984375" customWidth="1"/>
+    <col min="11" max="11" width="6.09765625" customWidth="1"/>
+    <col min="12" max="12" width="5.09765625" customWidth="1"/>
+    <col min="13" max="13" width="15.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="26" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" s="24" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="20"/>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="76" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="76"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="23"/>
+    </row>
+    <row r="2" spans="1:13" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A2" s="20"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+    </row>
+    <row r="3" spans="1:13" s="24" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A3" s="20"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+    </row>
+    <row r="4" spans="1:13" s="24" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="A4" s="20"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22"/>
+      <c r="J4" s="22"/>
+      <c r="K4" s="22"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="22"/>
+    </row>
+    <row r="5" spans="1:13" s="24" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="20"/>
+      <c r="B5" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="94"/>
+      <c r="D5" s="28"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="32"/>
+    </row>
+    <row r="6" spans="1:13" s="24" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="20"/>
+      <c r="B6" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="94"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="32"/>
+    </row>
+    <row r="7" spans="1:13" s="24" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="20"/>
+      <c r="B7" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="94"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="25"/>
+      <c r="M7" s="36"/>
     </row>
-    <row r="2" spans="1:14" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="20"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-    </row>
-    <row r="3" spans="1:14" s="26" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A3" s="20"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-    </row>
-    <row r="4" spans="1:14" s="26" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A4" s="20"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-    </row>
-    <row r="5" spans="1:14" s="26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20"/>
-      <c r="B5" s="30" t="s">
+    <row r="8" spans="1:13" s="24" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="20"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="M8" s="38"/>
+    </row>
+    <row r="9" spans="1:13" s="43" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39"/>
+      <c r="B9" s="40"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+    </row>
+    <row r="10" spans="1:13" s="43" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="31"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24"/>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="35" t="s">
+      <c r="B10" s="70" t="s">
         <v>22</v>
       </c>
-      <c r="N5" s="36">
-        <v>46021</v>
+      <c r="C10" s="81" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="83" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="84"/>
+      <c r="F10" s="85" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="86"/>
+      <c r="H10" s="87"/>
+      <c r="I10" s="70" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="72" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="73"/>
+      <c r="L10" s="88" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="88" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="20"/>
-      <c r="B6" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
-      <c r="G6" s="34"/>
-      <c r="H6" s="34"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="39" t="s">
-        <v>24</v>
-      </c>
-      <c r="N6" s="36"/>
-    </row>
-    <row r="7" spans="1:14" s="26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="20"/>
-      <c r="B7" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="30"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="N7" s="42"/>
-    </row>
-    <row r="8" spans="1:14" s="26" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="20"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="N8" s="44"/>
-    </row>
-    <row r="9" spans="1:14" s="49" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="45"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-    </row>
-    <row r="10" spans="1:14" s="49" customFormat="1" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="51" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="52" t="s">
+    <row r="11" spans="1:13" s="43" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="79"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="53"/>
-      <c r="E10" s="54" t="s">
+      <c r="E11" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="55"/>
-      <c r="G10" s="56" t="s">
+      <c r="F11" s="46" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="57"/>
-      <c r="I10" s="58"/>
-      <c r="J10" s="51" t="s">
+      <c r="H11" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="59" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" s="60"/>
-      <c r="M10" s="61" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" s="61" t="s">
-        <v>36</v>
-      </c>
+      <c r="I11" s="71"/>
+      <c r="J11" s="74"/>
+      <c r="K11" s="75"/>
+      <c r="L11" s="89"/>
+      <c r="M11" s="89"/>
     </row>
-    <row r="11" spans="1:14" s="49" customFormat="1" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="65"/>
-      <c r="E11" s="66" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="67" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="I11" s="70" t="s">
-        <v>40</v>
-      </c>
-      <c r="J11" s="71"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="74"/>
-      <c r="N11" s="74"/>
-    </row>
-    <row r="12" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="75">
+    <row r="12" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="49">
         <v>1</v>
       </c>
-      <c r="B12" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="76" t="s">
-        <v>3</v>
-      </c>
-      <c r="D12" s="77"/>
-      <c r="E12" s="14">
-        <v>80</v>
-      </c>
-      <c r="F12" s="78"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="80"/>
-      <c r="K12" s="81"/>
-      <c r="L12" s="82"/>
-      <c r="M12" s="83"/>
-      <c r="N12" s="84"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="51"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="53"/>
+      <c r="M12" s="54"/>
     </row>
-    <row r="13" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="75">
+    <row r="13" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="49">
         <v>2</v>
       </c>
       <c r="B13" s="14"/>
-      <c r="C13" s="76"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="86"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87"/>
-      <c r="J13" s="88"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="89"/>
-      <c r="M13" s="90"/>
-      <c r="N13" s="91"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="59"/>
     </row>
-    <row r="14" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="75">
+    <row r="14" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="49">
         <v>3</v>
       </c>
       <c r="B14" s="14"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="87"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="56"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="60"/>
       <c r="J14" s="92"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="90"/>
-      <c r="N14" s="93"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="58"/>
+      <c r="M14" s="61"/>
     </row>
-    <row r="15" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="75">
+    <row r="15" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="49">
         <v>4</v>
       </c>
       <c r="B15" s="14"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="86"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="95"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="96"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="56"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="62"/>
+      <c r="J15" s="92"/>
+      <c r="K15" s="92"/>
+      <c r="L15" s="58"/>
+      <c r="M15" s="63"/>
     </row>
-    <row r="16" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="75">
+    <row r="16" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="49">
         <v>5</v>
       </c>
       <c r="B16" s="14"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="97"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="87"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="95"/>
-      <c r="K16" s="89"/>
-      <c r="L16" s="89"/>
-      <c r="M16" s="90"/>
-      <c r="N16" s="91"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="55"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="56"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="62"/>
+      <c r="J16" s="92"/>
+      <c r="K16" s="92"/>
+      <c r="L16" s="58"/>
+      <c r="M16" s="59"/>
     </row>
-    <row r="17" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="75">
+    <row r="17" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="49">
         <v>6</v>
       </c>
       <c r="B17" s="14"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="86"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="95"/>
-      <c r="K17" s="89"/>
-      <c r="L17" s="89"/>
-      <c r="M17" s="90"/>
-      <c r="N17" s="91"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="62"/>
+      <c r="J17" s="92"/>
+      <c r="K17" s="92"/>
+      <c r="L17" s="58"/>
+      <c r="M17" s="59"/>
     </row>
-    <row r="18" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="75">
+    <row r="18" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="49">
         <v>7</v>
       </c>
       <c r="B18" s="14"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="97"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="98"/>
-      <c r="I18" s="98"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="89"/>
-      <c r="L18" s="89"/>
-      <c r="M18" s="90"/>
-      <c r="N18" s="91"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="64"/>
+      <c r="H18" s="64"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="58"/>
+      <c r="M18" s="59"/>
     </row>
-    <row r="19" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="75">
+    <row r="19" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="49">
         <v>8</v>
       </c>
       <c r="B19" s="14"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="94"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="87"/>
-      <c r="I19" s="87"/>
-      <c r="J19" s="95"/>
-      <c r="K19" s="89"/>
-      <c r="L19" s="89"/>
-      <c r="M19" s="90"/>
-      <c r="N19" s="96"/>
+      <c r="C19" s="97"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="56"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="92"/>
+      <c r="K19" s="92"/>
+      <c r="L19" s="58"/>
+      <c r="M19" s="63"/>
     </row>
-    <row r="20" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="75">
+    <row r="20" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="49">
         <v>9</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="97"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="87"/>
-      <c r="I20" s="87"/>
-      <c r="J20" s="95"/>
-      <c r="K20" s="89"/>
-      <c r="L20" s="89"/>
-      <c r="M20" s="90"/>
-      <c r="N20" s="91"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="55"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="56"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="92"/>
+      <c r="K20" s="92"/>
+      <c r="L20" s="58"/>
+      <c r="M20" s="59"/>
     </row>
-    <row r="21" spans="1:14" s="49" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="75">
+    <row r="21" spans="1:13" s="43" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="49">
         <v>10</v>
       </c>
       <c r="B21" s="14"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="97"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="86"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="87"/>
-      <c r="I21" s="87"/>
-      <c r="J21" s="95"/>
-      <c r="K21" s="89"/>
-      <c r="L21" s="89"/>
-      <c r="M21" s="90"/>
-      <c r="N21" s="91"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="17"/>
+      <c r="G21" s="56"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="92"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="58"/>
+      <c r="M21" s="59"/>
     </row>
-    <row r="22" spans="1:14" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="99"/>
-      <c r="B22" s="100" t="s">
-        <v>41</v>
+    <row r="22" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="65"/>
+      <c r="B22" s="93" t="s">
+        <v>34</v>
       </c>
-      <c r="C22" s="100"/>
-      <c r="D22" s="101"/>
-      <c r="E22" s="102">
-        <f>SUM(E12:E21)</f>
-        <v>80</v>
-      </c>
-      <c r="F22" s="102"/>
-      <c r="G22" s="102">
-        <f>SUM(G12:G21)</f>
+      <c r="C22" s="93"/>
+      <c r="D22" s="66">
+        <f>SUM(D12:D21)</f>
         <v>0</v>
       </c>
-      <c r="H22" s="102"/>
-      <c r="I22" s="102">
-        <f>SUM(I12:I21)</f>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66">
+        <f>SUM(F12:F21)</f>
         <v>0</v>
       </c>
-      <c r="J22" s="103"/>
-      <c r="K22" s="104"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="103"/>
-      <c r="N22" s="103"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66">
+        <f>SUM(H12:H21)</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="67"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="67"/>
+      <c r="M22" s="67"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="34" t="s">
-        <v>42</v>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B23" s="30" t="s">
+        <v>35</v>
       </c>
-      <c r="C23" s="34"/>
+      <c r="C23" s="98"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="K20:L20"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:L11"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="L10:L11"/>
     <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:K11"/>
+    <mergeCell ref="B1:F1"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:D11"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.74777776002883911" right="0.19666667282581329" top="0.27541667222976685" bottom="0.27541667222976685" header="0.23597222566604614" footer="0.15722222626209259"/>

</xml_diff>